<commit_message>
Modificada lectura de fichero maestro y fichero de datos
</commit_message>
<xml_diff>
--- a/src/test/resources/agents.xlsx
+++ b/src/test/resources/agents.xlsx
@@ -3,18 +3,14 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iván\git\Loader_e3b\doc\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="435" windowWidth="25605" windowHeight="15480"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15585" windowHeight="3255"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="0" concurrentCalc="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -30,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>Nombre</t>
   </si>
@@ -117,13 +113,22 @@
   </si>
   <si>
     <t>spacex</t>
+  </si>
+  <si>
+    <t>Person</t>
+  </si>
+  <si>
+    <t>Sensor</t>
+  </si>
+  <si>
+    <t>Entity</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -135,6 +140,14 @@
       <u/>
       <sz val="11"/>
       <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -161,10 +174,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
@@ -449,7 +463,7 @@
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,8 +504,8 @@
       <c r="D2" t="s">
         <v>1</v>
       </c>
-      <c r="E2">
-        <v>1</v>
+      <c r="E2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -507,15 +521,15 @@
       <c r="D3" t="s">
         <v>2</v>
       </c>
-      <c r="E3">
-        <v>1</v>
+      <c r="E3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="2" t="s">
@@ -524,8 +538,8 @@
       <c r="D4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E4">
-        <v>1</v>
+      <c r="E4" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -541,8 +555,8 @@
       <c r="D5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E5">
-        <v>3</v>
+      <c r="E5" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -558,8 +572,8 @@
       <c r="D6" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E6">
-        <v>2</v>
+      <c r="E6" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -575,8 +589,8 @@
       <c r="D7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7">
-        <v>3</v>
+      <c r="E7" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>